<commit_message>
Reajustes após verificações e modificações no prompt
</commit_message>
<xml_diff>
--- a/docs/respostas_classificacao_sentencas.xlsx
+++ b/docs/respostas_classificacao_sentencas.xlsx
@@ -472,7 +472,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>A empresa possuía madeira em tora sem licença válida, conforme Auto de Infração, configurando dano ambiental.</t>
+          <t>A empresa mantinha madeira ilegal em depósito, o que causa dano ambiental por fomentar a extração ilegal.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -493,7 +493,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sim, houve destruição de 121,15 hectares de floresta nativa no bioma amazônico sem autorização ambiental.</t>
+          <t>O texto refere-se à destruição de 121,15 hectares de floresta nativa, configurando dano ao meio ambiente.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -514,7 +514,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de uma ação de venda casada de carregadores de celular.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação judicial sobre a venda de um aparelho sem carregador.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -535,7 +535,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de interrupção no abastecimento de água e prejuízos decorrentes de vazamento.</t>
+          <t>Não há dano ambiental, pois o texto trata de interrupção no abastecimento de água e prejuízos econômicos.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de cobrança indevida de faturas de água por estimativa de consumo.</t>
+          <t>Não há dano ambiental. O texto trata de cobrança indevida de água, sem menção a prejuízos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -598,7 +598,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>O texto trata de uma ação judicial sobre cobrança indevida de IPTU, não mencionando danos ao meio ambiente.</t>
+          <t>Não há menção de prejuízo ao meio ambiente (água, solo, ar, fauna, flora, patrimônio paisagístico etc.) no texto.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de questões tributárias e indenização por danos morais.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação declaratória de inexistência de débito c/c reparação de danos morais.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -640,7 +640,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Não há informações no texto que indiquem a ocorrência de dano ambiental.</t>
+          <t>Não há dano ambiental no texto, pois trata-se de uma ação cível sobre compra e venda de veículo.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de questões financeiras e contratuais, sem menção a danos ao meio ambiente.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação judicial sobre um contrato de empréstimo.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -682,7 +682,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de ação declaratória de inexistência de débito c/c indenização por dano moral.</t>
+          <t>Não há dano ambiental, pois o texto trata de uma ação declaratória de inexistência de débito c/c indenização por dano moral.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de uma ação de rescisão contratual e restituição de valores pagos.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação de rescisão contratual sem relação com o meio ambiente.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -724,7 +724,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>O texto menciona uma ação civil pública por dano ambiental, indicando alteração na cobertura vegetal não justificada por perícia.</t>
+          <t>A ação civil pública trata de dano moral difuso e obrigação de recompor área degradada, indicando a existência de dano ambiental.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -745,7 +745,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Há dano ambiental devido à contaminação de rios e supressão de castanheiras, impactando comunidades indígenas e o ecossistema local.</t>
+          <t>O texto indica contaminação de rios, derrubada de castanheiras e poluição, caracterizando dano ambiental.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Houve desmatamento de 133,11 hectares de Floresta Amazônica sem autorização, afetando o equilíbrio do ecossistema e a biodiversidade.</t>
+          <t>O texto relata desmatamento ilegal de 133,11 hectares de Floresta Amazônica, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -787,7 +787,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>A empresa lançou efluentes industriais sem tratamento no Córrego Tamanduá, causando danos à fauna e flora locais.</t>
+          <t>A empresa lançou efluentes (tinta, produtos químicos e de limpeza) diretamente no solo e no Córrego Tamanduá, causando poluição.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -808,7 +808,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação ordinária inominada sobre direitos trabalhistas de uma professora municipal gestante.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação ordinária inominada sobre direitos trabalhistas de uma professora.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de indenização por danos morais devido a atraso de voo.</t>
+          <t>Não há dano ambiental, pois o texto trata de uma ação de indenização por danos morais devido a atraso de voo.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -850,7 +850,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental, pois o texto trata de um cumprimento de sentença e extinção do processo.</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -867,11 +867,11 @@
         <v>2451722545</v>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Sim, a interrupção do fornecimento de energia causou danos materiais e morais, afetando atividades empresariais e o bem-estar.</t>
+          <t>Não há dano ambiental, pois o texto trata de indenização por falhas no fornecimento de energia elétrica.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -892,7 +892,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental, pois o texto trata de uma ação de indenização por danos morais e materiais.</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de uma ação de indenização por danos materiais e morais.</t>
+          <t>Não há dano ambiental.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de uma ação de indenização por descumprimento de contrato de viagem.</t>
+          <t>Não há dano ambiental, pois o texto trata de descumprimento contratual referente a um pacote de viagem.</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -955,7 +955,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental, pois o texto trata de uma ação de restituição de valor pago c/c indenização por danos morais.</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -997,7 +997,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de cobranças indevidas de água e esgoto, configurando dano ao consumidor.</t>
+          <t>O texto trata de cobranças indevidas de água e esgoto, não mencionando danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Não há menção de dano ambiental no texto fornecido. O texto trata de questões de saúde e planos de saúde.</t>
+          <t>Não há dano ambiental, pois o texto trata de uma ação judicial sobre plano de saúde.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Construção irregular em área de praia causa poluição e degradação, afetando a balneabilidade e a saúde pública.</t>
+          <t>A construção irregular em área de praia (bem de uso comum) causa degradação ambiental, com potencial poluição e prejuízo à saúde pública.</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1060,7 +1060,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de uma disputa contratual entre um banco e um cliente.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação judicial sobre contrato de cartão de crédito consignado.</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Em 2016, a igreja emitia ruído acima dos limites tolerados, impactando moradores, conforme autos de infração ambiental nº 00537/2016 e 00485/2016.</t>
+          <t>Em 2016, houve emissão de ruído acima do aceitável para área residencial, causando transtornos aos moradores do entorno.</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1098,11 +1098,11 @@
         <v>779612317</v>
       </c>
       <c r="C32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Houve divergências entre o que foi vendido (área de lazer) e o que foi entregue (área de trabalho do condomínio).</t>
+          <t>Não há dano ambiental, pois o texto trata de rescisão de contrato de compra e venda de imóvel.</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Não há menção de dano ambiental no texto, apenas discussão sobre danos materiais e morais decorrentes de um acidente.</t>
+          <t>Não há dano ambiental. O texto trata de ação de indenização por danos materiais e morais em acidente de trânsito.</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de questões contratuais e financeiras de um contrato de locação comercial.</t>
+          <t>Não há informações no texto que permitam identificar dano ambiental.</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de ação declaratória de inexistência de débito.</t>
+          <t>O texto não descreve danos ao meio ambiente, mas sim uma ação declaratória de inexistência de débito.</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de descontos indevidos em benefício previdenciário e fraude bancária, sem menção ao meio ambiente.</t>
+          <t>Não há dano ambiental no texto, pois trata-se de ação declaratória sobre empréstimos não contratados e indenização por danos morais.</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Não há menção de dano ambiental no texto, que trata de rescisão de contrato de compra e venda de imóvel.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação de rescisão de contrato de compra e venda de imóvel.</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Não há menção de dano ambiental no texto, que trata de rescisão de contrato de compra e venda de imóvel.</t>
+          <t>Não há dano ambiental. O texto trata de rescisão de contrato de compra e venda de imóvel e questões financeiras.</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de rescisão contratual e reintegração de posse de imóvel.</t>
+          <t>Não há dano ambiental, pois o texto trata de rescisão contratual de compra e venda de imóvel.</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>O texto trata de rescisão de contrato de compra e venda, sem menção a danos ao meio ambiente.</t>
+          <t>Não há dano ambiental, pois o texto trata de rescisão de contrato de compra e venda de imóvel por inadimplência.</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Não há dano ambiental no texto, pois trata-se de uma ação cível sobre contrato de cartão de crédito.</t>
+          <t>Não há dano ambiental, pois o texto trata de questão financeira entre um banco e um cliente.</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de cobrança indevida de IPTU e dano moral.</t>
+          <t>Não há dano ambiental. O texto trata de cobrança indevida de IPTU e dano moral, não de prejuízo ao meio ambiente.</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação de reparação de danos por cobrança indevida de IPTU.</t>
+          <t>Não há dano ambiental. O texto trata de cobrança indevida de IPTU e dano moral, sem relação com o meio ambiente.</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>O texto trata de descumprimento contratual e dano moral, não mencionando dano ambiental.</t>
+          <t>Não há dano ambiental. O texto trata de atraso na entrega de obras e indenização por danos morais.</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1396,7 +1396,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>A não implantação da rede de esgoto sanitário e o uso de fossa séptica pode poluir o solo e as águas.</t>
+          <t>A ausência de rede de esgoto sanitário e o uso de fossa séptica podem poluir o solo e as águas.</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de reparação de danos morais por cobrança indevida de IPTU.</t>
+          <t>Não há dano ambiental, pois o texto trata de cobrança indevida de IPTU e dano moral, sem relação com o meio ambiente.</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de questões financeiras e contratuais, sem menção a danos ao meio ambiente.</t>
+          <t>O texto trata de questões financeiras e contratuais, não mencionando danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>O comprometimento do serviço de fornecimento de água, com uso de poços comunitários, indica dano aos recursos hídricos.</t>
+          <t>O texto demonstra comprometimento no fornecimento de água, recurso essencial ao meio ambiente e à população, configurando dano.</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1476,11 +1476,11 @@
         <v>2643510342</v>
       </c>
       <c r="C50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>O texto descreve o comprometimento do serviço de fornecimento de água, essencial à saúde e ao meio ambiente.</t>
+          <t>O texto trata de reparação por danos morais devido ao abastecimento irregular de água, não mencionando danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>O rompimento do encanamento que causou a interrupção do fornecimento de água configura dano ambiental.</t>
+          <t>O rompimento de encanamento causou interrupção no fornecimento de água, impactando o meio ambiente e a população.</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1522,7 +1522,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto se refere a um cumprimento de sentença cível.</t>
+          <t>Não há dano ambiental, pois o texto se refere a um cumprimento de sentença extinto, sem menção a danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Não há dano ambiental aparente no texto, que se refere a uma ata de audiência judicial.</t>
+          <t>Não há dano ambiental, pois o texto se refere a uma certidão de juntada de ata de audiência.</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>O texto relata desmate de 11,826 hectares de Mata Atlântica sem autorização, confirmando o dano ambiental.</t>
+          <t>O texto relata desmate de 11,826 hectares de Floresta Estacional Semidecidual do Bioma Mata Atlântica sem autorização.</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Houve supressão de 30 árvores nativas sem autorização, impactando a biodiversidade e inibindo a regeneração da vegetação.</t>
+          <t>Houve supressão de 30 árvores nativas, perda de biodiversidade e destruição de habitats, causando impacto ambiental negativo.</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>A construtora realizou captação irregular de água do Rio Verde, causando dano ambiental pontual, de pequena monta, aos recursos hídricos.</t>
+          <t>A construtora realizou captação irregular de água do Rio Verde, causando dano ambiental pontual, ainda que de pequena monta.</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Não há menção de dano ambiental no texto, apenas discussões sobre cláusulas contratuais e cobranças indevidas.</t>
+          <t>Não há dano ambiental. O texto trata de questões contratuais e financeiras entre as partes, sem menção a danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação de indenização por venda de produto impróprio para consumo.</t>
+          <t>O texto não menciona danos ao meio ambiente, apenas a venda de produtos vencidos.</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -1669,7 +1669,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental, pois o texto trata de uma ação declaratória de inexistência de débito c/c indenização por dano moral.</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de descontos indevidos em benefício previdenciário e dano moral.</t>
+          <t>Não há dano ambiental. O texto trata de descontos indevidos em benefício previdenciário, sem menção a danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação de indenização por danos morais devido à inscrição indevida no SISBACEN/SCR.</t>
+          <t>Não há dano ambiental, pois o texto trata de ação declaratória de inexistência de débito c/c reparação de danos morais.</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Não há menção a dano ambiental no texto, que trata de rescisão contratual e reintegração de posse.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação de rescisão contratual de compra e venda de imóvel.</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Não há menção de dano ambiental no texto fornecido. O texto trata de uma ação cível de inexistência de débito.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação declaratória de inexistência de débito c/c indenização por danos morais.</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação de indenização por danos morais devido à inclusão indevida no SISBACEN/SCR.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação de obrigação de fazer c/c indenização por dano extrapatrimonial.</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -1795,7 +1795,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Não há menção de dano ambiental no texto fornecido. O texto trata de uma ação de rescisão contratual.</t>
+          <t>Não há dano ambiental, pois o texto trata de rescisão contratual e danos materiais, sem menção a prejuízos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -1812,11 +1812,11 @@
         <v>1521765137</v>
       </c>
       <c r="C66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de ação de indenização por danos materiais decorrente de acidente de trânsito.</t>
+          <t>O acidente de trânsito causou danos materiais ao veículo, o que configura dano ao patrimônio, conforme artigos 186 e 927 do Código Civil.</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Não há menção a dano ambiental no texto, que trata de rescisão contratual e serviços financeiros.</t>
+          <t>Não há dano ambiental no texto, pois trata-se de uma ação de rescisão contratual.</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -1858,7 +1858,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Não foi comprovado dano ambiental resultante do depósito de resíduos de aves diretamente no solo, conforme o texto.</t>
+          <t>Apesar da infração administrativa, não foi comprovado dano ambiental resultante do depósito de resíduos de aves diretamente no solo.</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -1879,7 +1879,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de responsabilidade civil do estado por lesões causadas por disparo de arma de fogo.</t>
+          <t>Não há dano ambiental, pois o texto trata de responsabilidade civil do Estado por lesões causadas por um agente policial.</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -1900,7 +1900,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação de indenização por danos morais devido à inscrição indevida no SCR.</t>
+          <t>Não há dano ambiental. O texto trata de inscrição indevida no Sistema de Informações de Crédito do Banco Central (SCR).</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de erro médico em cirurgia plástica, sem menção a danos ao meio ambiente.</t>
+          <t>Não há dano ambiental. O texto trata de erro médico em cirurgia plástica, sem menção a prejuízos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Não há dano ambiental no texto, pois se refere a uma ação de reparação por danos morais e materiais.</t>
+          <t>O texto trata de uma ação de reparação por danos morais e materiais, não mencionando danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de uma ação de indenização por acidente de trânsito.</t>
+          <t>O texto se refere a uma ação de indenização por danos decorrentes de acidente de trânsito, sem menção a danos ambientais.</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -1984,7 +1984,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Não há dano ambiental no texto, pois este se refere a uma ação declaratória sobre contrato bancário.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação judicial sobre descontos não autorizados em benefício previdenciário.</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2005,7 +2005,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental. O texto trata de descontos não autorizados em benefício previdenciário, sem relação com o meio ambiente.</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2026,7 +2026,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de rescisão de contrato de compra e venda de móveis planejados.</t>
+          <t>Não há dano ambiental. O texto trata de um processo de rescisão contratual por desacordo comercial.</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2047,7 +2047,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de ação declaratória de inexistência de débito c/c indenização por danos morais.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação declaratória de inexistência de débito e indenização por danos morais.</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação de rescisão de contrato de compra e venda de móveis planejados.</t>
+          <t>Não há dano ambiental, pois o texto trata de uma ação de rescisão contratual e indenização por danos morais.</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2089,7 +2089,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de fraude bancária e indenização por danos morais e materiais.</t>
+          <t>O texto trata de fraude bancária e dano moral, não mencionando prejuízos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2110,7 +2110,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de ação declaratória de nulidade contratual c/c reparação por danos morais e materiais.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação declaratória de nulidade contratual e reparação por danos morais.</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de cobranças indevidas e danos morais, sem menção a questões ambientais.</t>
+          <t>Não há dano ambiental no texto, pois trata-se de ação declaratória de inexistência de débito c/c danos morais.</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental no texto, pois o caso trata de questões administrativas e de direito do consumidor.</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2173,7 +2173,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de ação de indenização por cobrança indevida c/c danos morais.</t>
+          <t>O texto trata de cobrança indevida e danos morais, sem menção a prejuízos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2215,7 +2215,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de inscrição indevida no Sistema de Informação de Crédito – SCR.</t>
+          <t>Não há dano ambiental, pois o texto trata de inscrição indevida no Sistema de Informação de Crédito, não envolvendo danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação de obrigação de fazer c/c indenização por danos morais.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação de indenização por danos morais devido à inclusão indevida no SISBACEN/SCR.</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2257,7 +2257,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação de indenização por cobrança indevida de IPTU.</t>
+          <t>Não há dano ambiental. O texto trata de ação de indenização por cobrança indevida de IPTU, sem relação com o meio ambiente.</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2278,7 +2278,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>O texto menciona a colisão de um veículo com um poste de energia elétrica, causando dano ambiental.</t>
+          <t>O texto relata colisão de veículo com poste de energia elétrica, caracterizando dano ao patrimônio paisagístico e à infraestrutura urbana.</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Não há menção de dano ambiental no texto, que trata de ação declaratória de inexistência de débitos c/c danos morais.</t>
+          <t>Não há dano ambiental no texto, pois trata-se de ação declaratória de inexistência de débitos c/c danos morais.</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -2320,7 +2320,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Não há dano ambiental aparente no texto, pois se trata de uma certidão judicial eletrônica.</t>
+          <t>Não há dano ambiental, pois o texto é uma certidão judicial sem informações sobre danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>O texto descreve degradação ambiental por aterramento de nascente e intervenção em APP, resultando em autos de infração.</t>
+          <t>A empresa causou degradação ambiental ao aterrar nascente e intervir em APP, conforme relatório técnico e autos de infração.</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -2362,7 +2362,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Houve intervenção em APP com assoreamento do Córrego Canta Galo, causado por deslizamento de terra, causando erosão no local.</t>
+          <t>Houve intervenção em APP com assoreamento do Córrego Canta Galo, causando erosão e prejuízo ao meio ambiente.</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -2383,7 +2383,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Houve intervenção em APP, causando erosão e assoreamento do Córrego Canta Galo, com prejuízo ao meio ambiente.</t>
+          <t>Houve erosão, assoreamento do córrego e intervenção em área de preservação permanente (APP) devido à construção do mineroduto.</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -2404,7 +2404,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de cumprimento de sentença sobre fornecimento de água e inclusão indevida em cadastro.</t>
+          <t>Não há dano ambiental, pois o texto se refere a um processo sobre fornecimento de água e inclusão indevida em cadastro.</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Houve destruição de 2.158,2727 hectares de floresta nativa na Região Amazônica entre 2009 e 2012 sem licença.</t>
+          <t>O texto informa sobre a destruição de 2.158,2727 hectares de floresta nativa na Região Amazônica, sem licença.</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Há indícios de fraudes em matrículas, títulos falsos e ocupação ilegal de terras, indicando dano ambiental.</t>
+          <t>Sim, pois há fortes indícios de títulos de propriedade falsos, impactando a regularidade fundiária e a destinação das terras.</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de questões processuais de uma ação civil pública.</t>
+          <t>O texto apenas informa sobre uma ação civil pública, sem mencionar dano ambiental.</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -2509,7 +2509,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de questões financeiras e de direito do consumidor.</t>
+          <t>Não há dano ambiental. O texto trata de descontos indevidos em conta corrente, não mencionando danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -2530,7 +2530,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação judicial sobre a invasão de uma conta no Facebook.</t>
+          <t>Não há dano ambiental no texto, pois este se refere a uma ação judicial sobre direito do consumidor.</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -2551,7 +2551,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de descontos indevidos em benefício previdenciário.</t>
+          <t>Não há dano ambiental no texto, pois trata-se de ação declaratória de nulidade de relação jurídica c/c pedido indenizatório.</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de indenização por negativação indevida, sem menção a danos ao meio ambiente.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação de indenização por negativação indevida, sem menção a danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de descontos indevidos em benefício previdenciário, sem menção a questões ambientais.</t>
+          <t>O texto trata de descontos indevidos em benefício previdenciário, sem relação com dano ao meio ambiente.</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -2614,7 +2614,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>O rompimento da barragem causou danos à fauna, flora, rede fluvial, solo, paisagem e economia local, configurando dano ambiental.</t>
+          <t>O rompimento da barragem causou danos à fauna, flora, rede fluvial, solo e paisagem, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto se refere a uma certidão de juntada de ata de audiência.</t>
+          <t>Não há dano ambiental, pois o texto se refere a um processo judicial sem menção a danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Houve desmate de 7 hectares de Floresta Decidual com tipologia do Bioma Mata Atlântica, sem autorização.</t>
+          <t>O texto relata desmate de 7 hectares de floresta decidual do Bioma Mata Atlântica sem autorização, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -2677,7 +2677,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Não há informações no texto que permitam identificar a ocorrência de dano ambiental.</t>
+          <t>Não há dano ambiental, pois o texto se refere a um processo judicial sem relação aparente com o meio ambiente.</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -2698,7 +2698,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Houve supressão de vegetação em área de preservação permanente e construção de barragem que causou a extinção de curso d’água.</t>
+          <t>O texto relata supressão de vegetação em APP e construção de barragem que extinguiu curso d’água, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -2719,7 +2719,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>O texto menciona depredação de área de preservação histórica e cultural, configurando dano ao patrimônio cultural e ambiental.</t>
+          <t>O texto relata depredação de bem de valor histórico e cultural, com consequente lesão ao meio ambiente cultural.</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -2740,7 +2740,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>O texto relata desmatamento de 118,58 hectares de floresta nativa sem autorização, configurando dano ambiental.</t>
+          <t>Sim, o texto descreve desmatamento de 118,58 hectares de floresta nativa sem autorização, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Sim, a inserção de informações falsas no SISFLORA/PA causou dano ambiental, com afetação da biota.</t>
+          <t>Sim, a inserção de informações falsas no SISFLORA/PA gerou créditos de madeira nativa indevidos, afetando a biota.</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -2782,7 +2782,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Sim, houve dano ambiental. A empresa inseriu informações falsas no sistema SISFLORA/PA, recebendo créditos florestais indevidos.</t>
+          <t>Sim, a MADEIREIRA NORDESTINA LTDA inseriu informações falsas no SISFLORA/PA, causando dano ambiental.</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -2803,7 +2803,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>A inserção de informações falsas no SISFLORA gerou créditos florestais indevidos, afetando a biota da Amazônia.</t>
+          <t>Sim, a inserção de informações falsas no SISFLORA gerou créditos florestais indevidos, afetando a biota da Amazônia.</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -2824,7 +2824,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Houve dano ambiental, pois o requerido impediu a regeneração natural de 8,61 hectares de vegetação nativa.</t>
+          <t>Houve impedimento da regeneração natural de 8,61 hectares de vegetação nativa, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -2845,7 +2845,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>A chácara vendida era área de preservação ambiental, configurando dano.</t>
+          <t>O texto menciona a venda de chácara em área de preservação ambiental, configurando dano ao meio ambiente.</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -2866,7 +2866,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de um processo cível sobre um serviço de desentupimento.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação de restituição de valores e indenização por danos morais.</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -2887,7 +2887,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de um processo de reparação de danos materiais e morais.</t>
+          <t>Não há dano ambiental, pois o texto trata de um processo de compra e venda de veículo.</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -2908,7 +2908,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de ação de ressarcimento de danos materiais c/c dano moral.</t>
+          <t>Não há dano ambiental, pois o texto se refere a uma ação de ressarcimento de danos materiais sem menção a dano ambiental.</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>A venda de madeira sem guia florestal válida configura dano ambiental, conforme o texto.</t>
+          <t>A venda de madeira sem guia florestal válida configura dano ambiental, sujeita à reparação, conforme legislação.</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -2950,7 +2950,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto se refere a uma sessão de conciliação em um processo judicial.</t>
+          <t>Não há dano ambiental, pois o texto se refere a uma ação judicial de natureza cível.</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -2971,7 +2971,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>A empresa adquiriu créditos florestais fictícios para acobertar madeira ilegal, resultando em desmatamento de 33,59825 hectares.</t>
+          <t>Sim, houve dano ambiental. A empresa adquiriu créditos florestais fictícios para acobertar madeira de origem clandestina, degradando 33,59825 hectares.</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -2992,7 +2992,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Sim, houve supressão de vegetação rasteira em APP e barramento sem autorização, além de erosão.</t>
+          <t>Sim, houve intervenção ambiental irregular em área de preservação permanente, com supressão de vegetação e danos aos recursos hídricos.</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -3013,7 +3013,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Não há dano ambiental no texto, pois o caso trata de apreensão e leilão de veículo.</t>
+          <t>O texto trata de indenização por danos materiais e morais, não mencionando danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -3034,7 +3034,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>A extração de sal-gema pela Braskem causou risco de desabamento/afundamento no bairro do Pinheiro, configurando dano ambiental.</t>
+          <t>A extração de sal-gema pela Braskem causou risco de desabamento/afundamento no bairro do Pinheiro, dano ao meio ambiente.</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -3055,7 +3055,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação de indenização por falha na prestação de serviços de fornecimento de água.</t>
+          <t>Não há dano ambiental, pois o texto se refere a uma ação de indenização por falha na prestação de serviços.</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -3076,7 +3076,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Sim, o lixão causou poluição da água, do solo e do ar, além de incêndios e morte de animais.</t>
+          <t>Sim, o lixão causou poluição do ar, contaminação do solo e da água, além de morte de animais.</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -3097,7 +3097,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de negativação indevida e indenização por danos morais.</t>
+          <t>Não há dano ambiental, pois o texto trata de uma ação de indenização por danos morais, sem relação com o meio ambiente.</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -3118,7 +3118,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de relação de consumo e cobranças indevidas.</t>
+          <t>Não há dano ambiental. O texto trata de cobranças indevidas em serviços de telefonia e internet.</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -3135,11 +3135,11 @@
         <v>1873600114</v>
       </c>
       <c r="C129" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Há dano ambiental devido ao vazamento de dados de saúde de usuários, conforme mencionado nos embargos de declaração.</t>
+          <t>Não há dano ambiental. O texto trata de embargos de declaração sobre vazamento de dados de saúde.</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -3160,7 +3160,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Não há dano ambiental no texto, pois ele se refere a um sistema eletrônico judicial.</t>
+          <t>Não há dano ambiental aparente no texto, que se limita a instruções de acesso ao sistema PJe.</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -3181,7 +3181,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de rescisão de contrato de compra e venda de imóvel.</t>
+          <t>O texto trata de rescisão de contrato de compra e venda, sem menção a danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -3202,7 +3202,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de mandado de segurança sobre tratamento de saúde.</t>
+          <t>Não há dano ambiental. O texto trata de um mandado de segurança sobre um procedimento cirúrgico negado.</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -3244,7 +3244,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>O texto relata supressão irregular de vegetação da Floresta Amazônica, configurando dano ambiental.</t>
+          <t>O texto refere-se à supressão irregular de vegetação da Floresta Amazônica, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -3261,11 +3261,11 @@
         <v>1369683877</v>
       </c>
       <c r="C135" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>A falta de fornecimento de água tratada, essencial à vida, configura dano ambiental, impactando a dignidade humana e a saúde.</t>
+          <t>Não há dano ambiental, pois o texto se refere a falha na prestação de serviço de fornecimento de água.</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -3286,7 +3286,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação de indenização por descumprimento de contrato de compra de passagens aéreas.</t>
+          <t>Não há dano ambiental, pois o texto trata de questões de direito do consumidor, sem menção a prejuízos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -3307,7 +3307,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto se refere à destruição de uma barraca de frutas em um passeio público.</t>
+          <t>Não há dano ambiental, pois o dano é material à barraca e não ao meio ambiente.</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -3328,7 +3328,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto se refere a um processo cível sobre indenização por dano moral e material.</t>
+          <t>Não há dano ambiental, pois o texto se refere a um procedimento do Juizado Especial Cível.</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>A supressão do carregador não internaliza custos ambientais, transferindo-os ao consumidor, sem ganho ambiental mensurável.</t>
+          <t>A supressão do carregador de bateria não internaliza custos ambientais, transferindo a responsabilidade da poluição para o consumidor.</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -3370,7 +3370,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental, pois o texto se refere a um processo sobre vendas casadas e indenização por dano moral.</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -3391,7 +3391,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Não há menção a dano ambiental no texto, apenas a um acidente de trânsito e suas consequências.</t>
+          <t>Não há dano ambiental, pois o texto se refere a um acidente de trânsito e suas consequências para os envolvidos.</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -3412,7 +3412,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Sim, houve movimentação de terra, efetuação de cavas e outras atividades que degradaram o meio ambiente.</t>
+          <t>Sim, houve movimentação de terra e cavas sem recuperação da flora, além de erosões em direção às nascentes.</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>O texto menciona autuações e ações contra empresas de fundição por irregularidades ambientais.</t>
+          <t>O texto menciona autuações devido a irregularidades ambientais em empresas de fundição, indicando dano ambiental.</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
@@ -3454,7 +3454,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>O lançamento de efluentes industriais em desacordo com os parâmetros legais causou poluição hídrica, configurando dano ambiental.</t>
+          <t>Sim, houve lançamento de efluentes em desacordo com os padrões normativos, causando dano ambiental, conforme auto de infração.</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -3475,7 +3475,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>O texto descreve desmatamento ilegal para produção de carvão vegetal, caracterizando dano ao meio ambiente.</t>
+          <t>O texto indica desmatamento de 2,62 hectares para cada carga de carvão, configurando dano à flora e ao bioma.</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -3496,7 +3496,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Sim, devido à supressão de vegetação nativa e movimentação de terra em Área de Preservação Permanente (APP).</t>
+          <t>Sim, o texto demonstra a supressão de vegetação nativa em APP e movimentação de terra em loteamento irregular.</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -3513,11 +3513,11 @@
         <v>2496355003</v>
       </c>
       <c r="C147" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Quedas de energia causam prejuízos econômicos e podem afetar a integridade física e a vida de cidadãos.</t>
+          <t>Não há dano ambiental. O texto trata de problemas no fornecimento de energia elétrica, sem menção a danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -3538,7 +3538,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>O rompimento de cabo elétrico causou curto-circuito, faíscas e incêndio que queimaram 33,40 hectares de pastagem, configurando dano ambiental.</t>
+          <t>O rompimento de cabo de energia causou curto-circuito e incêndio, queimando 33,40 hectares de pastagem, dano ao meio ambiente.</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -3559,7 +3559,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>O texto narra lançamento de resíduos líquidos e funcionamento de serviços poluidores sem licença, causando potencial dano à saúde.</t>
+          <t>O texto menciona lançamento de resíduos líquidos e substâncias oleosas em desacordo com a lei, causando poluição.</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
@@ -3580,7 +3580,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>A queda da ponte causou degradação ambiental no Rio Santo Antônio, como o assoreamento e prejuízo à reprodução de peixes.</t>
+          <t>A queda da ponte causou obstrução do leito do rio, assoreamento e prejuízo à reprodução de peixes, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -3601,7 +3601,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Os relatórios de vistoria e o laudo técnico de 2013 comprovam o dano ambiental por erosão, assoreamento e acesso do gado.</t>
+          <t>Sim, pois há processos erosivos que contribuem para o assoreamento do rio, além de morte da mata ciliar.</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -3622,7 +3622,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Não há menção de dano ambiental no texto fornecido. O texto trata de um processo judicial.</t>
+          <t>Não há dano ambiental, pois o texto trata de um processo judicial sem menção a danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -3643,7 +3643,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>O texto trata de descontos indevidos em benefício previdenciário, não mencionando danos ao meio ambiente.</t>
+          <t>Não há dano ambiental. O texto trata de descontos indevidos em benefício previdenciário e dano moral.</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -3664,7 +3664,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de ação de reparação por danos materiais e morais devido a atraso de voo.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação de reparação por danos materiais e morais devido a atraso de voo.</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -3685,7 +3685,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de uma ação de indenização por danos materiais e morais.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação de indenização por danos materiais e morais devido a um atraso de voo.</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -3706,7 +3706,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de uma ação de indenização por danos morais.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação declaratória de inexistência de débito e indenização por danos morais.</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
@@ -3727,7 +3727,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>O uso inadequado de agrotóxicos, sem respeitar a distância mínima, causou prejuízos à saúde e ao meio ambiente.</t>
+          <t>O texto descreve aplicação inadequada de agrotóxicos, contaminando plantações vizinhas e causando prejuízos aos moradores da região.</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -3748,7 +3748,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de um processo sobre consórcio e questões financeiras.</t>
+          <t>Não há dano ambiental. O texto trata de um processo sobre consórcio e não menciona danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -3769,7 +3769,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>Sim, pois a área do terreno é considerada de preservação permanente devido à existência de uma mina d’água.</t>
+          <t>O texto menciona a existência de uma mina d’água em área de preservação permanente, impedindo a construção no local.</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>A empresa foi autuada por lançar resíduos líquidos em desacordo com as normas, o que resultou em dano ambiental.</t>
+          <t>A empresa foi multada e condenada por lançar resíduos em desacordo com a lei, causando dano ambiental.</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -3811,7 +3811,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental, pois o texto trata de ação de indenização por problemas com voo.</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
@@ -3832,7 +3832,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>Sim, a manutenção ilegal em cativeiro e a comercialização de aves silvestres configuram dano ambiental.</t>
+          <t>Sim, a manutenção ilegal em cativeiro e comercialização de aves silvestres configura dano ambiental, conforme o texto.</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
@@ -3853,7 +3853,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o caso trata de negligência médica e dano moral, sem menção a impactos no meio ambiente.</t>
+          <t>Não há dano ambiental, pois o texto trata de erro médico e indenização por danos morais, sem menção a prejuízos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há referência a dano ambiental no texto fornecido.</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -3891,11 +3891,11 @@
         <v>1124177887</v>
       </c>
       <c r="C165" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>Há menção a Ação Civil Pública e Indenização por Dano Moral, indicando potencial dano ambiental a ser apurado.</t>
+          <t>O texto se refere a um processo sobre inversão do ônus da prova, sem menção a danos ambientais.</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
@@ -3916,7 +3916,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental, pois o texto trata de um acidente de trânsito e indenizações decorrentes, sem menção a danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
@@ -3937,7 +3937,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>O laudo pericial constatou supressão de floresta nativa na área de servidão, danificando o meio ambiente.</t>
+          <t>Houve supressão de floresta nativa para a passagem dos cabos de energia, causando danos ambientais na área de servidão.</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
@@ -3958,7 +3958,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto se refere a uma homologação de acordo em processo judicial.</t>
+          <t>Não há dano ambiental, pois o texto se refere a uma homologação de acordo.</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
@@ -3979,7 +3979,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>O texto menciona desmatamento ilegal na área da Fazenda São Judas, configurando dano ambiental.</t>
+          <t>O texto informa que houve desmatamento ilegal na área incorporada pela Fazenda São Judas, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
@@ -4021,7 +4021,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto se refere a um cumprimento de sentença judicial.</t>
+          <t>Não há dano ambiental. O texto trata de um cumprimento de sentença judicial entre Gilberto e o Banco do Brasil.</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -4042,7 +4042,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de questões tributárias e de execução fiscal, não envolvendo degradação do meio ambiente.</t>
+          <t>O texto não descreve prejuízo ao meio ambiente, mas sim um erro administrativo com implicações financeiras para o autor.</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
@@ -4063,7 +4063,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>O texto trata de acidente de trânsito e não menciona danos ao meio ambiente.</t>
+          <t>O texto trata de um acidente de trânsito e não especifica danos ao meio ambiente, como poluição ou destruição de recursos naturais.</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
@@ -4084,7 +4084,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental, pois o texto trata de uma ação rescisória e restituição de valores por perdas financeiras.</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
@@ -4105,7 +4105,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>O texto indica irregularidades ambientais na propriedade rural, como ausência de reserva legal averbada e alterações ambientais por barragem.</t>
+          <t>O texto demonstra alteração ambiental com a implantação de represa em área úmida, necessitando de readequação e licenciamento.</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
@@ -4126,7 +4126,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Construção de casas em área de preservação permanente da Mata Atlântica, com destruição de vegetação nativa.</t>
+          <t>Construção de residências em área de preservação permanente da Mata Atlântica, com supressão de vegetação nativa.</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
@@ -4147,7 +4147,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Houve erosão do solo, contaminação e assoreamento do leito do rio Ribeirão do Tigre por omissão na manutenção de galerias.</t>
+          <t>Houve erosão do solo e contaminação do rio, causados pela falta de manutenção das galerias de águas pluviais.</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
@@ -4189,7 +4189,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Houve dano ambiental devido ao vazamento de esgoto que causou danos estruturais à propriedade, necessitando demolição e reconstrução.</t>
+          <t>Houve vazamento de esgoto, causando danos estruturais em imóvel devido à saturação do solo, afetando o meio ambiente.</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -4210,7 +4210,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Sim, devido à degradação da mata ciliar, erosão das margens do córrego Caviúna e assoreamento dos rios.</t>
+          <t>A degradação da mata ciliar e a erosão causada pelas águas pluviais caracterizam dano ambiental, com obrigação de reparação.</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -4231,7 +4231,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>O texto menciona que o terreno estava embargado devido a problemas ambientais, impossibilitando qualquer construção.</t>
+          <t>O texto menciona embargo do terreno devido a problemas ambientais, impossibilitando construção, o que configura dano ambiental.</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
@@ -4252,7 +4252,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o caso trata da perda de um animal de estimação em um aeroporto.</t>
+          <t>Não há dano ambiental, pois o texto trata de extravio de animal de estimação, sem menção a prejuízos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
@@ -4273,7 +4273,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Construção em área de preservação permanente e impedimento de regeneração de vegetação nativa configuram dano ambiental.</t>
+          <t>Construção em área de preservação permanente impediu a regeneração da vegetação nativa, causando degradação ambiental.</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
@@ -4294,7 +4294,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Há dano ambiental devido à supressão de vegetação nativa em área de preservação permanente para construção de garagem náutica.</t>
+          <t>O texto menciona supressão de vegetação nativa de Mata Atlântica e construção em área de preservação permanente.</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
@@ -4315,7 +4315,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de indenização por danos materiais e morais devido a questões contratuais.</t>
+          <t>Não há dano ambiental, pois o texto trata de indenização por danos materiais e morais devido a um contrato de aluguel de carro.</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -4336,7 +4336,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>A instalação inadequada de depósitos de materiais excedentes causou enchentes e alagamentos recorrentes, gerando sérios prejuízos à população.</t>
+          <t>A instalação inadequada de depósitos de materiais excedentes causou enchentes e alagamentos recorrentes, com sérios prejuízos à população e ao meio ambiente.</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
@@ -4357,7 +4357,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>A escavação causou a liberação de gases tóxicos, contaminando a água e causando a mortandade de peixes no Rio Cubatão.</t>
+          <t>A escavação do leito do rio causou a liberação de gases tóxicos, contaminando a água e causando a morte de peixes.</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
@@ -4378,7 +4378,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>O texto demonstra degradação ambiental em floresta ombrófila densa, através de desmatamento e construção, confirmado por Auto de Infração Ambiental.</t>
+          <t>Sim, houve desmatamento e construção em área de floresta ombrófila densa, causando degradação ambiental, conforme o texto.</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
@@ -4399,7 +4399,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Houve poluição de cursos d'água por extravasamento de esgoto sanitário sem tratamento adequado, afetando a fauna e a população local.</t>
+          <t>Houve poluição de cursos d'água por extravasamento de esgoto sanitário, afetando a fauna marinha e tornando a região imprópria para banho.</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
@@ -4420,7 +4420,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Os réus destruíram vegetação nativa em área de preservação permanente, sem autorização, causando dano ambiental.</t>
+          <t>Sim, houve destruição de vegetação nativa em área de preservação permanente, sem autorização dos órgãos ambientais competentes.</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
@@ -4441,7 +4441,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>A conduta da ré praticamente obriga a compra de milhares de carregadores novos, aumentando os impactos climáticos.</t>
+          <t>A prática da empresa obriga a compra de milhares de carregadores novos, aumentando os impactos climáticos e gerando mais lucro.</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
@@ -4462,7 +4462,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Omissão do município permitiu desmatamento em área de mata atlântica, construções sem licenças e em locais de risco de inundações.</t>
+          <t>Omissão do município permite desmatamentos em área de mata atlântica e construções irregulares em áreas de risco de inundações.</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
@@ -4483,7 +4483,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Não há dano ambiental. O texto trata de ação indenizatória por atraso na entrega de imóvel.</t>
+          <t>Não há dano ambiental, pois o texto trata de ação indenizatória referente a atraso na entrega de imóvel.</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
@@ -4504,7 +4504,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Sim, a alteração na composição do vermífugo causou intoxicação e morte de filhotes, afetando a fauna.</t>
+          <t>Sim, a contaminação por vermífugo adulterado causou a morte de vários filhotes, configurando dano à fauna.</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
@@ -4525,7 +4525,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de uma ação judicial referente a um plano de saúde.</t>
+          <t>Não há dano ambiental no texto, pois ele trata de uma ação judicial sobre cobertura de plano de saúde.</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental, pois o texto trata de agressão verbal e física, não de prejuízo ao meio ambiente.</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
@@ -4567,7 +4567,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de uma ação sobre plano de saúde.</t>
+          <t>Não há dano ambiental, pois o texto trata de uma disputa sobre um plano de saúde.</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
@@ -4588,7 +4588,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental. O texto trata de questões contratuais e de prestação de serviços, sem menção a danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
@@ -4609,7 +4609,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de cobranças indevidas e dano moral ao consumidor.</t>
+          <t>Não há dano ambiental, pois o texto trata de cobranças indevidas e dano moral, sem relação com o meio ambiente.</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
@@ -4651,7 +4651,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>O texto trata de uma ação judicial sobre contratos financeiros, sem menção a danos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
@@ -4672,7 +4672,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>O texto refere-se à destruição de floresta amazônica e uso ilegal de bem público em reserva extrativista.</t>
+          <t>Sim, houve desmatamento desordenado e criação de gado em área de reserva extrativista, impactando o meio ambiente.</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
@@ -4693,7 +4693,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>O texto menciona destruição de floresta amazônica e uso ilegal de bem público, caracterizando dano ambiental.</t>
+          <t>O texto indica desmatamento desordenado de grande área de vegetação em área de Reserva Extrativista, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
@@ -4714,7 +4714,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de uma ação judicial sobre plano de saúde.</t>
+          <t>Não há dano ambiental, pois o texto trata de uma disputa contratual relacionada a um plano de saúde.</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
@@ -4735,7 +4735,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>O terreno encontra-se em área de proteção ambiental, impossibilitando a construção e causando dano ao meio ambiente.</t>
+          <t>O terreno encontra-se em área de proteção ambiental, o que caracteriza dano ao meio ambiente.</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
@@ -4756,7 +4756,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de agressão física em jogo de futebol, com indenização por dano moral.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação de indenização por dano moral devido a agressão física.</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
@@ -4777,7 +4777,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto se refere a um processo judicial sobre embargos de declaração.</t>
+          <t>Não há menção de prejuízo ao meio ambiente no texto fornecido.</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
@@ -4798,7 +4798,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de questões financeiras envolvendo compra e venda de criptomoedas.</t>
+          <t>Não há dano ambiental. O texto trata de uma ação judicial sobre compra e venda de criptomoedas.</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
@@ -4819,7 +4819,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de fraude bancária e indenização por danos morais.</t>
+          <t>Não há dano ambiental. O texto trata de ação de restituição de valor c/c indenização por dano moral decorrente de fraude bancária.</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
@@ -4840,7 +4840,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>O funcionário aplicava herbicidas sem proteção, colocando em risco a saúde e causando dano ambiental.</t>
+          <t>O funcionário aplicava herbicidas sem proteção, colocando sua saúde em risco. Isso afeta a saúde humana, que é parte do meio ambiente.</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>O texto menciona "atividade sonora sem autorização ambiental", indicando dano ao meio ambiente sonoro.</t>
+          <t>A emissão de atividade sonora sem autorização ambiental é dano ao meio ambiente, conforme exposto no texto.</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
@@ -4882,7 +4882,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há dano ambiental, pois o texto se refere a multa por descumprimento do Código de Defesa do Consumidor.</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
@@ -4903,7 +4903,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>A árvore causa rachaduras e risco de desabamento, conforme laudo técnico, indicando dano ao meio ambiente urbano.</t>
+          <t>A árvore causou rachaduras no calçamento e fissuras no muro, danificando o meio ambiente urbano.</t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
@@ -4924,7 +4924,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de extravio de mercadorias e questões comerciais.</t>
+          <t>Não há dano ambiental. O texto trata de extravio de mercadorias e questões contratuais, sem menção a prejuízos ao meio ambiente.</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de um acidente de trânsito e suas consequências legais.</t>
+          <t>Não há dano ambiental. O texto trata de um acidente de trânsito e suas consequências para os envolvidos.</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
@@ -4966,7 +4966,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Não há dano ambiental, pois o texto trata de uma ação de indenização por acidente de trânsito.</t>
+          <t>Não há dano ambiental, pois o texto trata de um acidente de trânsito e suas consequências legais.</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
@@ -4987,7 +4987,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>Não há dano ambiental.</t>
+          <t>Não há menção de prejuízo ao meio ambiente no texto fornecido. O texto trata de negligência de um advogado.</t>
         </is>
       </c>
       <c r="E217" t="inlineStr">
@@ -5008,7 +5008,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>O texto indica que o loteamento está em área de preservação permanente, nascentes e várzeas, com risco de desabamento.</t>
+          <t>O texto relata construção em área de preservação permanente, com risco de desabamento, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E218" t="inlineStr">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>Há alagamento e infiltração no imóvel, e a locadora não realizou os reparos no telhado, podendo causar danos ambientais.</t>
+          <t>Há menção de danos no imóvel, decorrente de alagamento e infiltração por problemas no telhado, conforme fls. 1787, 1788.</t>
         </is>
       </c>
       <c r="E219" t="inlineStr">
@@ -5071,7 +5071,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>O texto informa sobre desmatamento ilegal de 422,58 hectares na Amazônia Legal, configurando dano ambiental.</t>
+          <t>O texto descreve desmatamento ilegal de 422,58 hectares na Amazônia Legal, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E221" t="inlineStr">
@@ -5092,7 +5092,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>Houve desmatamento ilegal de 71,9 hectares de floresta primária na região amazônica, configurando dano ambiental.</t>
+          <t>Houve desmatamento ilegal de 71,9 hectares de floresta primária na Amazônia, configurando dano ambiental.</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>O texto se limita a discutir ressarcimento patrimonial por extração de calcário sem autorização, não abordando dano ambiental.</t>
+          <t>Não há pedido de ressarcimento de suposto dano ambiental no texto fornecido, apenas de ressarcimento patrimonial.</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
@@ -5130,11 +5130,11 @@
         <v>1787605420</v>
       </c>
       <c r="C224" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>O texto menciona ressarcimento ao erário por extração de calcário sem autorização, não havendo pedido de reparação por dano ambiental.</t>
+          <t>Foi constatada extração de calcário sem autorização, o que configura dano ambiental ao solo e ao patrimônio da União.</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">

</xml_diff>